<commit_message>
update sore tgl 25
</commit_message>
<xml_diff>
--- a/STOK DEALER/STOK BHG.xlsx
+++ b/STOK DEALER/STOK BHG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Wanda - PSD\HIL\HIL 2025\STOK DEALER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03EB040-B0B5-4268-8976-EC6533D9659D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA13DF1-0987-4B80-9A0B-64BF8198E776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69DFFCF3-4EBB-4C5E-9380-5C22F317BD78}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{69DFFCF3-4EBB-4C5E-9380-5C22F317BD78}"/>
   </bookViews>
   <sheets>
     <sheet name="STOK DEALER" sheetId="1" r:id="rId1"/>
@@ -14399,13 +14399,13 @@
         <v>64</v>
       </c>
       <c r="F96" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G96" s="2">
         <v>0</v>
       </c>
       <c r="H96" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -14581,10 +14581,10 @@
         <v>64</v>
       </c>
       <c r="F103" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H103" s="2">
         <v>413</v>
@@ -14893,13 +14893,13 @@
         <v>64</v>
       </c>
       <c r="F115" s="2">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="G115" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H115" s="2">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -14997,13 +14997,13 @@
         <v>64</v>
       </c>
       <c r="F119" s="2">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="G119" s="2">
         <v>0</v>
       </c>
       <c r="H119" s="2">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -15101,10 +15101,10 @@
         <v>64</v>
       </c>
       <c r="F123" s="2">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G123" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H123" s="2">
         <v>106</v>
@@ -19911,10 +19911,10 @@
         <v>64</v>
       </c>
       <c r="F308" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G308" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H308" s="2">
         <v>16</v>
@@ -22927,10 +22927,10 @@
         <v>813</v>
       </c>
       <c r="F424" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G424" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H424" s="2">
         <v>4</v>
@@ -24825,10 +24825,10 @@
         <v>946</v>
       </c>
       <c r="F497" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G497" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H497" s="2">
         <v>6</v>
@@ -54829,13 +54829,13 @@
         <v>64</v>
       </c>
       <c r="F1651" s="2">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G1651" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H1651" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="1652" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>